<commit_message>
commit code UI + logic
</commit_message>
<xml_diff>
--- a/listPage.xlsx
+++ b/listPage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB\WebQRCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4D0AC1-3E1D-43CC-83D8-2C13D74B1841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7ADE8F-08B0-453F-95F2-E5CB23B4E1BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Page</t>
   </si>
@@ -57,9 +57,6 @@
     <t>- Add category</t>
   </si>
   <si>
-    <t>bill</t>
-  </si>
-  <si>
     <t>Account</t>
   </si>
   <si>
@@ -88,6 +85,15 @@
   </si>
   <si>
     <t>-Edit Staff</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>order Detail</t>
+  </si>
+  <si>
+    <t>order</t>
   </si>
 </sst>
 </file>
@@ -190,6 +196,8 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -199,11 +207,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:E12"/>
+  <dimension ref="C4:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -496,91 +502,102 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="3:6" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="3:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="C5" s="5" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="3:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="C6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="3:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="3:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="C7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="C8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="C9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="3:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="3:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="C11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>